<commit_message>
add check purchase order permission structure
</commit_message>
<xml_diff>
--- a/src/main/resources/uploadfile/import_location_receipt/import_location_receipt_template.xlsx
+++ b/src/main/resources/uploadfile/import_location_receipt/import_location_receipt_template.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20361"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\GoSELL-Automation-Local\src\main\resources\uploadfile\import_location_receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3107B8-973B-41E4-9647-481426130C64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9109806-DF2D-4AA2-B28F-BBF5B54C999E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Product ID</t>
   </si>
@@ -40,56 +40,22 @@
     <t>1</t>
   </si>
   <si>
-    <t>328</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>1248154-1240599</t>
   </si>
   <si>
-    <t>[vi1] Auto - Normal - Variation - 02/11 11:23:34</t>
-  </si>
-  <si>
     <t>[vi] Auto - Normal - Variation - 02/11 11:23:34</t>
   </si>
   <si>
-    <t>1277792-1281649</t>
-  </si>
-  <si>
-    <t>[vi] Auto - Normal - variation - 01/02 16:56:10</t>
-  </si>
-  <si>
-    <t>1709519810912</t>
-  </si>
-  <si>
-    <t>1710215117211</t>
-  </si>
-  <si>
-    <t>1710215205264</t>
-  </si>
-  <si>
-    <t>1710215486920</t>
-  </si>
-  <si>
-    <t>354</t>
-  </si>
-  <si>
-    <t>355</t>
-  </si>
-  <si>
-    <t>364</t>
-  </si>
-  <si>
-    <t>1710216596271</t>
+    <t>366</t>
+  </si>
+  <si>
+    <t>1710302702850</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -416,15 +382,15 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.88671875"/>
-    <col min="2" max="2" customWidth="true" width="16.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.33203125"/>
-    <col min="5" max="5" customWidth="true" width="10.33203125"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -445,20 +411,20 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>20</v>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">

</xml_diff>

<commit_message>
fix some issue when update product
</commit_message>
<xml_diff>
--- a/src/main/resources/uploadfile/import_location_receipt/import_location_receipt_template.xlsx
+++ b/src/main/resources/uploadfile/import_location_receipt/import_location_receipt_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20361"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\GoSELL-Automation-Local\src\main\resources\uploadfile\import_location_receipt\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="27">
   <si>
     <t>Product ID</t>
   </si>
@@ -50,12 +50,64 @@
   </si>
   <si>
     <t>1710302702850</t>
+  </si>
+  <si>
+    <t>406</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1254198-1245711</t>
+  </si>
+  <si>
+    <t>[vi] Auto - Normal - Variation - 02/01 09:58:19</t>
+  </si>
+  <si>
+    <t>1712130520703</t>
+  </si>
+  <si>
+    <t>407</t>
+  </si>
+  <si>
+    <t>408</t>
+  </si>
+  <si>
+    <t>1712134102426</t>
+  </si>
+  <si>
+    <t>1712134553982</t>
+  </si>
+  <si>
+    <t>1712134930118</t>
+  </si>
+  <si>
+    <t>412</t>
+  </si>
+  <si>
+    <t>413</t>
+  </si>
+  <si>
+    <t>1712139645990</t>
+  </si>
+  <si>
+    <t>416</t>
+  </si>
+  <si>
+    <t>1712140120951</t>
+  </si>
+  <si>
+    <t>1712140330995</t>
+  </si>
+  <si>
+    <t>1712140573166</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -387,10 +439,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.88671875"/>
+    <col min="2" max="2" customWidth="true" width="16.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.33203125"/>
+    <col min="5" max="5" customWidth="true" width="10.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -411,20 +463,16 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="0"/>
+      <c r="B2" s="0"/>
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="D2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5">

</xml_diff>